<commit_message>
added missing file name in excel, added feature in chemcode - in chemfiles.xlsx: added reation 17 imine scope substrate 1 entry 7 - in chemcode: added distance method to molecule
</commit_message>
<xml_diff>
--- a/chemfiles.xlsx
+++ b/chemfiles.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlisd\Downloads\chem_brandeis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B4D3D1-C865-45ED-A4E1-0292C4B18AB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3031" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3032" uniqueCount="494">
   <si>
     <t>reaction</t>
   </si>
@@ -1501,8 +1507,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1565,6 +1571,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1611,7 +1625,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1643,9 +1657,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1677,6 +1709,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1852,14 +1902,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I445"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
+      <selection activeCell="F372" sqref="F372"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="37.21875" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1885,7 +1942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1911,7 +1968,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1937,7 +1994,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1963,7 +2020,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1989,7 +2046,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2015,7 +2072,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2041,7 +2098,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2067,7 +2124,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2093,7 +2150,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2119,7 +2176,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2145,7 +2202,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2171,7 +2228,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2197,7 +2254,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2223,7 +2280,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2249,7 +2306,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2275,7 +2332,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2301,7 +2358,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2327,7 +2384,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2353,7 +2410,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2379,7 +2436,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2405,7 +2462,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2434,7 +2491,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2463,7 +2520,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2492,7 +2549,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2521,7 +2578,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2550,7 +2607,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2579,7 +2636,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2608,7 +2665,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2637,7 +2694,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2666,7 +2723,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2695,7 +2752,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2724,7 +2781,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2753,7 +2810,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2782,7 +2839,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2811,7 +2868,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2840,7 +2897,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2869,7 +2926,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2898,7 +2955,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2927,7 +2984,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2956,7 +3013,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2985,7 +3042,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3014,7 +3071,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3043,7 +3100,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3072,7 +3129,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3101,7 +3158,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3130,7 +3187,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3159,7 +3216,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3188,7 +3245,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3217,7 +3274,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3246,7 +3303,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3275,7 +3332,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3304,7 +3361,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3333,7 +3390,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3362,7 +3419,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3391,7 +3448,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3420,7 +3477,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3449,7 +3506,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3478,7 +3535,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3507,7 +3564,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3536,7 +3593,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3565,7 +3622,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3594,7 +3651,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3623,7 +3680,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3652,7 +3709,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3681,7 +3738,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3710,7 +3767,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3739,7 +3796,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3768,7 +3825,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3797,7 +3854,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3826,7 +3883,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3855,7 +3912,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3884,7 +3941,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3913,7 +3970,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3942,7 +3999,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3971,7 +4028,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4000,7 +4057,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4029,7 +4086,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4058,7 +4115,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4087,7 +4144,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4116,7 +4173,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4145,7 +4202,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4174,7 +4231,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -4203,7 +4260,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -4232,7 +4289,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4261,7 +4318,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4290,7 +4347,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4319,7 +4376,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4348,7 +4405,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4377,7 +4434,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4406,7 +4463,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4435,7 +4492,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4464,7 +4521,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4493,7 +4550,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4522,7 +4579,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4551,7 +4608,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4580,7 +4637,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4609,7 +4666,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4638,7 +4695,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4667,7 +4724,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4696,7 +4753,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4725,7 +4782,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4754,7 +4811,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -4783,7 +4840,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -4812,7 +4869,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -4841,7 +4898,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -4870,7 +4927,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -4899,7 +4956,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -4928,7 +4985,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -4957,7 +5014,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -4986,7 +5043,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -5015,7 +5072,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -5044,7 +5101,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -5073,7 +5130,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -5102,7 +5159,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -5131,7 +5188,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -5160,7 +5217,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -5189,7 +5246,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -5218,7 +5275,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -5247,7 +5304,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -5276,7 +5333,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -5305,7 +5362,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -5334,7 +5391,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -5363,7 +5420,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -5392,7 +5449,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -5421,7 +5478,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -5450,7 +5507,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -5479,7 +5536,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -5508,7 +5565,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -5537,7 +5594,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -5566,7 +5623,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -5595,7 +5652,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -5624,7 +5681,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -5653,7 +5710,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -5682,7 +5739,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -5711,7 +5768,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -5740,7 +5797,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -5769,7 +5826,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -5798,7 +5855,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -5827,7 +5884,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -5856,7 +5913,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -5885,7 +5942,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -5914,7 +5971,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -5943,7 +6000,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -5972,7 +6029,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -6001,7 +6058,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -6030,7 +6087,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -6059,7 +6116,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -6088,7 +6145,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -6117,7 +6174,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -6146,7 +6203,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -6175,7 +6232,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -6204,7 +6261,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -6233,7 +6290,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -6262,7 +6319,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -6291,7 +6348,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -6320,7 +6377,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -6349,7 +6406,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -6378,7 +6435,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -6407,7 +6464,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -6436,7 +6493,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -6465,7 +6522,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -6494,7 +6551,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -6523,7 +6580,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -6552,7 +6609,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -6581,7 +6638,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -6610,7 +6667,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -6639,7 +6696,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="168" spans="1:9">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -6668,7 +6725,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -6697,7 +6754,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -6726,7 +6783,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -6755,7 +6812,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -6784,7 +6841,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -6813,7 +6870,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -6842,7 +6899,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -6871,7 +6928,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -6900,7 +6957,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="177" spans="1:9">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -6929,7 +6986,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="178" spans="1:9">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -6958,7 +7015,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="179" spans="1:9">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -6987,7 +7044,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -7016,7 +7073,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="181" spans="1:9">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -7045,7 +7102,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="182" spans="1:9">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -7074,7 +7131,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="183" spans="1:9">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -7103,7 +7160,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="184" spans="1:9">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -7132,7 +7189,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -7161,7 +7218,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="186" spans="1:9">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -7190,7 +7247,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="187" spans="1:9">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -7219,7 +7276,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -7248,7 +7305,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="189" spans="1:9">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -7277,7 +7334,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="190" spans="1:9">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -7306,7 +7363,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="191" spans="1:9">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -7335,7 +7392,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="192" spans="1:9">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -7364,7 +7421,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="193" spans="1:9">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -7393,7 +7450,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="194" spans="1:9">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -7422,7 +7479,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="195" spans="1:9">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -7451,7 +7508,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="196" spans="1:9">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -7480,7 +7537,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="197" spans="1:9">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -7509,7 +7566,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="198" spans="1:9">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -7538,7 +7595,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="199" spans="1:9">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -7567,7 +7624,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="200" spans="1:9">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -7596,7 +7653,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -7625,7 +7682,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="202" spans="1:9">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -7654,7 +7711,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="203" spans="1:9">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -7683,7 +7740,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -7712,7 +7769,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="205" spans="1:9">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -7741,7 +7798,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="206" spans="1:9">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -7770,7 +7827,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="207" spans="1:9">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -7799,7 +7856,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -7828,7 +7885,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="209" spans="1:9">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -7857,7 +7914,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="210" spans="1:9">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -7886,7 +7943,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -7915,7 +7972,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -7944,7 +8001,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -7973,7 +8030,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -8002,7 +8059,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -8031,7 +8088,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -8060,7 +8117,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -8089,7 +8146,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -8118,7 +8175,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -8147,7 +8204,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="220" spans="1:9">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -8176,7 +8233,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="221" spans="1:9">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -8205,7 +8262,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -8234,7 +8291,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -8263,7 +8320,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -8292,7 +8349,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -8321,7 +8378,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -8350,7 +8407,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -8379,7 +8436,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="228" spans="1:9">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -8408,7 +8465,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -8437,7 +8494,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -8466,7 +8523,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -8495,7 +8552,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -8524,7 +8581,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -8553,7 +8610,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -8582,7 +8639,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -8611,7 +8668,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -8640,7 +8697,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="237" spans="1:9">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -8669,7 +8726,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="238" spans="1:9">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -8698,7 +8755,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="239" spans="1:9">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -8727,7 +8784,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="240" spans="1:9">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -8756,7 +8813,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="241" spans="1:9">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -8785,7 +8842,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="242" spans="1:9">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -8814,7 +8871,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -8843,7 +8900,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="244" spans="1:9">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -8872,7 +8929,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="245" spans="1:9">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -8901,7 +8958,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="246" spans="1:9">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -8930,7 +8987,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="247" spans="1:9">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -8959,7 +9016,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -8988,7 +9045,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="249" spans="1:9">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -9017,7 +9074,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="250" spans="1:9">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -9046,7 +9103,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="251" spans="1:9">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -9075,7 +9132,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="252" spans="1:9">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -9104,7 +9161,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="253" spans="1:9">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -9133,7 +9190,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="254" spans="1:9">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -9162,7 +9219,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="255" spans="1:9">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -9191,7 +9248,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="256" spans="1:9">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -9220,7 +9277,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="257" spans="1:9">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -9249,7 +9306,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="258" spans="1:9">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -9278,7 +9335,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="259" spans="1:9">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -9307,7 +9364,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="260" spans="1:9">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -9336,7 +9393,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="261" spans="1:9">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -9365,7 +9422,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="262" spans="1:9">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -9394,7 +9451,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="263" spans="1:9">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -9423,7 +9480,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="264" spans="1:9">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -9452,7 +9509,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="265" spans="1:9">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -9481,7 +9538,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="266" spans="1:9">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -9510,7 +9567,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="267" spans="1:9">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -9539,7 +9596,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="268" spans="1:9">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -9568,7 +9625,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="269" spans="1:9">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -9597,7 +9654,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="270" spans="1:9">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -9626,7 +9683,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="271" spans="1:9">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -9655,7 +9712,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="272" spans="1:9">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -9684,7 +9741,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="273" spans="1:9">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -9713,7 +9770,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="274" spans="1:9">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -9742,7 +9799,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="275" spans="1:9">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -9771,7 +9828,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="276" spans="1:9">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -9800,7 +9857,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="277" spans="1:9">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -9829,7 +9886,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="278" spans="1:9">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -9858,7 +9915,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="279" spans="1:9">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -9887,7 +9944,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="280" spans="1:9">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -9916,7 +9973,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="281" spans="1:9">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -9945,7 +10002,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="282" spans="1:9">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -9974,7 +10031,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="283" spans="1:9">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -10003,7 +10060,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="284" spans="1:9">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -10032,7 +10089,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="285" spans="1:9">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -10061,7 +10118,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="286" spans="1:9">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -10090,7 +10147,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="287" spans="1:9">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -10119,7 +10176,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="288" spans="1:9">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -10148,7 +10205,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="289" spans="1:9">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -10177,7 +10234,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="290" spans="1:9">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -10206,7 +10263,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="291" spans="1:9">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -10235,7 +10292,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="292" spans="1:9">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -10264,7 +10321,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="293" spans="1:9">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -10293,7 +10350,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="294" spans="1:9">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -10322,7 +10379,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="295" spans="1:9">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -10351,7 +10408,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="296" spans="1:9">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -10380,7 +10437,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="297" spans="1:9">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -10409,7 +10466,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="298" spans="1:9">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -10438,7 +10495,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="299" spans="1:9">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -10467,7 +10524,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="300" spans="1:9">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -10496,7 +10553,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="301" spans="1:9">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -10525,7 +10582,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="302" spans="1:9">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -10554,7 +10611,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="303" spans="1:9">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -10583,7 +10640,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="304" spans="1:9">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -10612,7 +10669,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="305" spans="1:9">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -10641,7 +10698,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="306" spans="1:9">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -10670,7 +10727,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="307" spans="1:9">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -10699,7 +10756,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="308" spans="1:9">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -10728,7 +10785,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -10757,7 +10814,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="310" spans="1:9">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -10786,7 +10843,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="311" spans="1:9">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -10815,7 +10872,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="312" spans="1:9">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -10844,7 +10901,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="313" spans="1:9">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -10873,7 +10930,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="314" spans="1:9">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -10902,7 +10959,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="315" spans="1:9">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -10931,7 +10988,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="316" spans="1:9">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -10960,7 +11017,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="317" spans="1:9">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -10989,7 +11046,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="318" spans="1:9">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -11018,7 +11075,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="319" spans="1:9">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -11047,7 +11104,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="320" spans="1:9">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -11076,7 +11133,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="321" spans="1:9">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -11105,7 +11162,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="322" spans="1:9">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -11134,7 +11191,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="323" spans="1:9">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -11163,7 +11220,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="324" spans="1:9">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -11192,7 +11249,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="325" spans="1:9">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -11221,7 +11278,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="326" spans="1:9">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -11250,7 +11307,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="327" spans="1:9">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -11279,7 +11336,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="328" spans="1:9">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -11308,7 +11365,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="329" spans="1:9">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -11337,7 +11394,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="330" spans="1:9">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -11366,7 +11423,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -11395,7 +11452,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="332" spans="1:9">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -11424,7 +11481,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="333" spans="1:9">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -11453,7 +11510,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="334" spans="1:9">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -11482,7 +11539,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="335" spans="1:9">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -11511,7 +11568,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="336" spans="1:9">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -11540,7 +11597,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="337" spans="1:9">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -11569,7 +11626,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="338" spans="1:9">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -11598,7 +11655,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="339" spans="1:9">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -11627,7 +11684,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="340" spans="1:9">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -11656,7 +11713,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="341" spans="1:9">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -11685,7 +11742,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="342" spans="1:9">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -11714,7 +11771,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="343" spans="1:9">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -11743,7 +11800,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="344" spans="1:9">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -11772,7 +11829,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="345" spans="1:9">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -11801,7 +11858,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="346" spans="1:9">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -11830,7 +11887,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="347" spans="1:9">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -11859,7 +11916,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="348" spans="1:9">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -11888,7 +11945,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="349" spans="1:9">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -11917,7 +11974,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="350" spans="1:9">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -11946,7 +12003,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="351" spans="1:9">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -11975,7 +12032,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="352" spans="1:9">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -12004,7 +12061,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="353" spans="1:9">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -12033,7 +12090,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="354" spans="1:9">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -12062,7 +12119,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="355" spans="1:9">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -12091,7 +12148,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="356" spans="1:9">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -12120,7 +12177,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="357" spans="1:9">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -12149,7 +12206,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="358" spans="1:9">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -12178,7 +12235,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="359" spans="1:9">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -12207,7 +12264,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="360" spans="1:9">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -12236,7 +12293,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="361" spans="1:9">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -12265,7 +12322,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="362" spans="1:9">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -12294,7 +12351,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="363" spans="1:9">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -12323,7 +12380,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="364" spans="1:9">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -12352,7 +12409,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="365" spans="1:9">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -12381,7 +12438,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="366" spans="1:9">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -12410,7 +12467,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="367" spans="1:9">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -12439,7 +12496,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="368" spans="1:9">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -12468,7 +12525,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="369" spans="1:9">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -12497,7 +12554,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="370" spans="1:9">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -12526,7 +12583,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="371" spans="1:9">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -12555,7 +12612,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="372" spans="1:9">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -12584,7 +12641,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="373" spans="1:9">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -12613,7 +12670,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="374" spans="1:9">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -12642,7 +12699,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="375" spans="1:9">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -12655,6 +12712,9 @@
       <c r="D375">
         <v>7</v>
       </c>
+      <c r="E375" t="s">
+        <v>64</v>
+      </c>
       <c r="F375" t="s">
         <v>238</v>
       </c>
@@ -12668,7 +12728,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="376" spans="1:9">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -12697,7 +12757,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="377" spans="1:9">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -12726,7 +12786,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="378" spans="1:9">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -12755,7 +12815,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="379" spans="1:9">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -12784,7 +12844,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="380" spans="1:9">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -12813,7 +12873,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="381" spans="1:9">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -12842,7 +12902,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="382" spans="1:9">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -12868,7 +12928,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="383" spans="1:9">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -12894,7 +12954,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="384" spans="1:9">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -12920,7 +12980,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="385" spans="1:9">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -12946,7 +13006,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="386" spans="1:9">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A386" s="1">
         <v>384</v>
       </c>
@@ -12972,7 +13032,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="387" spans="1:9">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -12998,7 +13058,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="388" spans="1:9">
+    <row r="388" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -13024,7 +13084,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="389" spans="1:9">
+    <row r="389" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -13050,7 +13110,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="390" spans="1:9">
+    <row r="390" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -13076,7 +13136,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="391" spans="1:9">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -13102,7 +13162,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="392" spans="1:9">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -13128,7 +13188,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="393" spans="1:9">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -13154,7 +13214,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="394" spans="1:9">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A394" s="1">
         <v>392</v>
       </c>
@@ -13180,7 +13240,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="395" spans="1:9">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -13206,7 +13266,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="396" spans="1:9">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -13232,7 +13292,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="397" spans="1:9">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -13258,7 +13318,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="398" spans="1:9">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -13284,7 +13344,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="399" spans="1:9">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -13310,7 +13370,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="400" spans="1:9">
+    <row r="400" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -13336,7 +13396,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="401" spans="1:9">
+    <row r="401" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -13362,7 +13422,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="402" spans="1:9">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -13388,7 +13448,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="403" spans="1:9">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A403" s="1">
         <v>401</v>
       </c>
@@ -13414,7 +13474,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="404" spans="1:9">
+    <row r="404" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A404" s="1">
         <v>402</v>
       </c>
@@ -13440,7 +13500,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="405" spans="1:9">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A405" s="1">
         <v>403</v>
       </c>
@@ -13466,7 +13526,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="406" spans="1:9">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A406" s="1">
         <v>404</v>
       </c>
@@ -13492,7 +13552,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="407" spans="1:9">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -13518,7 +13578,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="408" spans="1:9">
+    <row r="408" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -13544,7 +13604,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="409" spans="1:9">
+    <row r="409" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A409" s="1">
         <v>407</v>
       </c>
@@ -13570,7 +13630,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="410" spans="1:9">
+    <row r="410" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A410" s="1">
         <v>408</v>
       </c>
@@ -13596,7 +13656,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="411" spans="1:9">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A411" s="1">
         <v>409</v>
       </c>
@@ -13622,7 +13682,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="412" spans="1:9">
+    <row r="412" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -13648,7 +13708,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="413" spans="1:9">
+    <row r="413" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A413" s="1">
         <v>411</v>
       </c>
@@ -13674,7 +13734,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="414" spans="1:9">
+    <row r="414" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -13700,7 +13760,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="415" spans="1:9">
+    <row r="415" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A415" s="1">
         <v>413</v>
       </c>
@@ -13726,7 +13786,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="416" spans="1:9">
+    <row r="416" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A416" s="1">
         <v>414</v>
       </c>
@@ -13752,7 +13812,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="417" spans="1:9">
+    <row r="417" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A417" s="1">
         <v>415</v>
       </c>
@@ -13778,7 +13838,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="418" spans="1:9">
+    <row r="418" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -13804,7 +13864,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="419" spans="1:9">
+    <row r="419" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A419" s="1">
         <v>417</v>
       </c>
@@ -13830,7 +13890,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="420" spans="1:9">
+    <row r="420" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A420" s="1">
         <v>418</v>
       </c>
@@ -13856,7 +13916,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="421" spans="1:9">
+    <row r="421" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A421" s="1">
         <v>419</v>
       </c>
@@ -13882,7 +13942,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="422" spans="1:9">
+    <row r="422" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -13908,7 +13968,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="423" spans="1:9">
+    <row r="423" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A423" s="1">
         <v>421</v>
       </c>
@@ -13934,7 +13994,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="424" spans="1:9">
+    <row r="424" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A424" s="1">
         <v>422</v>
       </c>
@@ -13960,7 +14020,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="425" spans="1:9">
+    <row r="425" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -13986,7 +14046,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="426" spans="1:9">
+    <row r="426" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A426" s="1">
         <v>424</v>
       </c>
@@ -14012,7 +14072,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="427" spans="1:9">
+    <row r="427" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A427" s="1">
         <v>425</v>
       </c>
@@ -14038,7 +14098,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="428" spans="1:9">
+    <row r="428" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A428" s="1">
         <v>426</v>
       </c>
@@ -14064,7 +14124,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="429" spans="1:9">
+    <row r="429" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A429" s="1">
         <v>427</v>
       </c>
@@ -14090,7 +14150,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="430" spans="1:9">
+    <row r="430" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A430" s="1">
         <v>428</v>
       </c>
@@ -14116,7 +14176,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="431" spans="1:9">
+    <row r="431" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A431" s="1">
         <v>429</v>
       </c>
@@ -14142,7 +14202,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="432" spans="1:9">
+    <row r="432" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -14168,7 +14228,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="433" spans="1:9">
+    <row r="433" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A433" s="1">
         <v>431</v>
       </c>
@@ -14194,7 +14254,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="434" spans="1:9">
+    <row r="434" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -14220,7 +14280,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="435" spans="1:9">
+    <row r="435" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A435" s="1">
         <v>433</v>
       </c>
@@ -14246,7 +14306,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="436" spans="1:9">
+    <row r="436" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A436" s="1">
         <v>434</v>
       </c>
@@ -14272,7 +14332,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="437" spans="1:9">
+    <row r="437" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A437" s="1">
         <v>435</v>
       </c>
@@ -14298,7 +14358,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="438" spans="1:9">
+    <row r="438" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A438" s="1">
         <v>436</v>
       </c>
@@ -14324,7 +14384,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="439" spans="1:9">
+    <row r="439" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A439" s="1">
         <v>437</v>
       </c>
@@ -14350,7 +14410,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="440" spans="1:9">
+    <row r="440" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A440" s="1">
         <v>438</v>
       </c>
@@ -14376,7 +14436,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="441" spans="1:9">
+    <row r="441" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A441" s="1">
         <v>439</v>
       </c>
@@ -14402,7 +14462,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="442" spans="1:9">
+    <row r="442" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A442" s="1">
         <v>440</v>
       </c>
@@ -14428,7 +14488,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="443" spans="1:9">
+    <row r="443" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A443" s="1">
         <v>441</v>
       </c>
@@ -14454,7 +14514,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="444" spans="1:9">
+    <row r="444" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A444" s="1">
         <v>442</v>
       </c>
@@ -14480,7 +14540,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="445" spans="1:9">
+    <row r="445" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A445" s="1">
         <v>443</v>
       </c>

</xml_diff>